<commit_message>
Some work on 23/09
</commit_message>
<xml_diff>
--- a/Temps de travail Théo.xlsx
+++ b/Temps de travail Théo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theophile_mt/Desktop/Work/Government of Vanuatu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7850077A-1387-6948-AF84-5AD4AA428AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470B7F0C-709C-6B40-B2EA-30AE77BA1E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{3F34E535-2AA7-A445-A0B0-8D2DDE077566}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20820" xr2:uid="{3F34E535-2AA7-A445-A0B0-8D2DDE077566}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,16 +415,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC21656-7C63-B943-ACFE-4A43BFBC33DF}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -451,6 +451,22 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45922</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45923</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>